<commit_message>
Archive / small fixed
</commit_message>
<xml_diff>
--- a/DreamDigger.xlsx
+++ b/DreamDigger.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0788705-EFC9-4DEC-8342-C096A6155CDF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F01262-5F1D-4C4A-8615-152319AC3387}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -232,6 +232,10 @@
   </si>
   <si>
     <t>老话说得好，步子太大，会扯到蛋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>记录存档逻辑</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -333,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -380,6 +384,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -660,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1047,6 +1052,14 @@
         <v>44</v>
       </c>
     </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="16">
+        <v>43528</v>
+      </c>
+      <c r="B46" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>